<commit_message>
Rebuilt and tested VGA system.  Software to select VGA mode remains to be updated
</commit_message>
<xml_diff>
--- a/Resources/Character ROM.xlsx
+++ b/Resources/Character ROM.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\N.I.G.E.-Machine\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2529394E-46DC-4E9E-B7F4-58FA94B0E8D6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="18195" windowHeight="6210" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="18195" windowHeight="6210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Display" sheetId="2" r:id="rId1"/>
@@ -17,7 +23,7 @@
     <sheet name="ASCII" sheetId="3" r:id="rId8"/>
     <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -1128,7 +1134,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1247,6 +1253,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1268,7 +1277,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3073" name="il_fi" descr="http://solarsystem.nasa.gov/multimedia/gallery/all_symbols-browse.jpg"/>
+        <xdr:cNvPr id="3073" name="il_fi" descr="http://solarsystem.nasa.gov/multimedia/gallery/all_symbols-browse.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-0000010C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1308,7 +1323,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1" descr="zodiac symbols"/>
+        <xdr:cNvPr id="1025" name="Picture 1" descr="zodiac symbols">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1379,7 +1400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1412,9 +1433,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1447,6 +1485,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1622,11 +1677,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,7 +1704,7 @@
         <v>33</v>
       </c>
       <c r="B1" s="3">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>34</v>
@@ -1664,7 +1719,7 @@
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B2">
         <f>B1+1</f>
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2">
         <v>128</v>
@@ -1767,33 +1822,33 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="1" t="str">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A4)</f>
-        <v>8</v>
+        <v>3c</v>
       </c>
       <c r="C4">
         <f>HEX2DEC(B4)</f>
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <f>MOD(C4,D$2)</f>
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:K4" si="0">MOD(D4,E$2)</f>
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
@@ -1932,37 +1987,37 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="str">
+      <c r="B5" s="1">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A5)</f>
-        <v>1c</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C11" si="4">HEX2DEC(B5)</f>
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:K5" si="5">MOD(C5,D$2)</f>
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="E5">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <f t="shared" si="5"/>
@@ -2065,33 +2120,33 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="str">
+      <c r="B6" s="1">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A6)</f>
-        <v>3e</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:K6" si="12">MOD(C6,D$2)</f>
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <f t="shared" si="12"/>
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="F6">
         <f t="shared" si="12"/>
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <f t="shared" si="12"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I6">
         <f t="shared" si="12"/>
@@ -2200,39 +2255,39 @@
       </c>
       <c r="B7" s="1" t="str">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A7)</f>
-        <v>7f</v>
+        <v>0c</v>
       </c>
       <c r="C7">
         <f t="shared" si="4"/>
-        <v>127</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:K7" si="15">MOD(C7,D$2)</f>
-        <v>127</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <f t="shared" si="15"/>
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <f t="shared" si="15"/>
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G7">
         <f t="shared" si="15"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H7">
         <f t="shared" si="15"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I7">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <f t="shared" si="15"/>
@@ -2331,41 +2386,41 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="str">
+      <c r="B8" s="1">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A8)</f>
-        <v>7f</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <f t="shared" si="4"/>
-        <v>127</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:K8" si="18">MOD(C8,D$2)</f>
-        <v>127</v>
+        <v>16</v>
       </c>
       <c r="E8">
         <f t="shared" si="18"/>
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="F8">
         <f t="shared" si="18"/>
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="G8">
         <f t="shared" si="18"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <f t="shared" si="18"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <f t="shared" si="18"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <f t="shared" si="18"/>
@@ -2464,33 +2519,33 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="str">
+      <c r="B9" s="1">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A9)</f>
-        <v>1c</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <f t="shared" ref="D9:K9" si="21">MOD(C9,D$2)</f>
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <f t="shared" si="21"/>
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <f t="shared" si="21"/>
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <f t="shared" si="21"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <f t="shared" si="21"/>
@@ -2597,37 +2652,37 @@
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="str">
+      <c r="B10" s="1">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A10)</f>
-        <v>3e</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <f t="shared" si="4"/>
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <f t="shared" ref="D10:K10" si="24">MOD(C10,D$2)</f>
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <f t="shared" si="24"/>
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="F10">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G10">
         <f t="shared" si="24"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <f t="shared" si="24"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <f t="shared" si="24"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <f t="shared" si="24"/>
@@ -2875,11 +2930,11 @@
       </c>
       <c r="F13" s="2">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="30"/>
@@ -2887,7 +2942,7 @@
       </c>
       <c r="I13" s="2">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="30"/>
@@ -2968,7 +3023,7 @@
       </c>
       <c r="E14" s="2">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="32"/>
@@ -2976,19 +3031,19 @@
       </c>
       <c r="G14" s="2">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="32"/>
@@ -3069,19 +3124,19 @@
       </c>
       <c r="F15" s="2">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="35"/>
@@ -3162,15 +3217,15 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="37"/>
@@ -3182,11 +3237,11 @@
       </c>
       <c r="J16" s="2">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="2"/>
       <c r="P16" s="2">
@@ -3259,11 +3314,11 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="39"/>
@@ -3271,19 +3326,19 @@
       </c>
       <c r="H17" s="2">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="2"/>
       <c r="P17" s="2">
@@ -3364,15 +3419,15 @@
       </c>
       <c r="G18" s="2">
         <f t="shared" si="41"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="41"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="41"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="41"/>
@@ -3457,7 +3512,7 @@
       </c>
       <c r="F19" s="2">
         <f t="shared" si="43"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="43"/>
@@ -3465,15 +3520,15 @@
       </c>
       <c r="H19" s="2">
         <f t="shared" si="43"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="43"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="43"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="2">
         <f t="shared" si="43"/>
@@ -5577,7 +5632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23820,7 +23875,7 @@
         <v>366</v>
       </c>
       <c r="Y194" t="str">
-        <f t="shared" ref="Y194:Y256" si="28">I194&amp;", "&amp;J194&amp;", "&amp;K194&amp;", "&amp;L194&amp;", "&amp;M194&amp;", "&amp;N194&amp;", "&amp;O194&amp;", "&amp;P194&amp;", "&amp;Q194&amp;", "&amp;R194&amp;", "&amp;S194&amp;", "&amp;T194&amp;", "&amp;U194&amp;", "&amp;V194&amp;", "&amp;W194&amp;", "&amp;X194&amp;", "</f>
+        <f t="shared" ref="Y194:Y255" si="28">I194&amp;", "&amp;J194&amp;", "&amp;K194&amp;", "&amp;L194&amp;", "&amp;M194&amp;", "&amp;N194&amp;", "&amp;O194&amp;", "&amp;P194&amp;", "&amp;Q194&amp;", "&amp;R194&amp;", "&amp;S194&amp;", "&amp;T194&amp;", "&amp;U194&amp;", "&amp;V194&amp;", "&amp;W194&amp;", "&amp;X194&amp;", "</f>
         <v xml:space="preserve">800, 800, 7E00, 800, 800, 1000, 2000, 000, 0000, 0000, 0000, 0000, 0000, 0000, 0000, 0000, </v>
       </c>
     </row>
@@ -29659,10 +29714,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V256"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
@@ -40986,7 +41041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -47662,7 +47717,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -54595,7 +54650,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S512"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -69659,7 +69714,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -76333,7 +76388,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B256"/>
   <sheetViews>
     <sheetView topLeftCell="A82" workbookViewId="0">
@@ -78656,7 +78711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Completed VGA rebuild, including changing 800x600 to 40MHz clock and other fine tuning To change mode: INCLUDE VGA.F VGA1 VGA2 VGA3 VGA4
</commit_message>
<xml_diff>
--- a/Resources/Character ROM.xlsx
+++ b/Resources/Character ROM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\N.I.G.E.-Machine\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2529394E-46DC-4E9E-B7F4-58FA94B0E8D6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F37392-CB1C-40F5-84A3-84BFE9A738DF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="18195" windowHeight="6210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1704,7 +1704,7 @@
         <v>33</v>
       </c>
       <c r="B1" s="3">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>34</v>
@@ -1719,7 +1719,7 @@
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B2">
         <f>B1+1</f>
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>128</v>
@@ -2122,15 +2122,15 @@
       </c>
       <c r="B6" s="1">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A6)</f>
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:K6" si="12">MOD(C6,D$2)</f>
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="E6">
         <f t="shared" si="12"/>
@@ -2255,23 +2255,23 @@
       </c>
       <c r="B7" s="1" t="str">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A7)</f>
-        <v>0c</v>
+        <v>3c</v>
       </c>
       <c r="C7">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:K7" si="15">MOD(C7,D$2)</f>
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E7">
         <f t="shared" si="15"/>
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="F7">
         <f t="shared" si="15"/>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="G7">
         <f t="shared" si="15"/>
@@ -2388,35 +2388,35 @@
       </c>
       <c r="B8" s="1">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A8)</f>
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:K8" si="18">MOD(C8,D$2)</f>
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="E8">
         <f t="shared" si="18"/>
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <f t="shared" si="18"/>
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="G8">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I8">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J8">
         <f t="shared" si="18"/>
@@ -2521,35 +2521,35 @@
       </c>
       <c r="B9" s="1">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A9)</f>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C9">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="D9">
         <f t="shared" ref="D9:K9" si="21">MOD(C9,D$2)</f>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E9">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I9">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J9">
         <f t="shared" si="21"/>
@@ -2652,33 +2652,33 @@
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="1" t="str">
         <f>INDEX('C64 ROM'!$A$1:$H$256,$B$2, A10)</f>
-        <v>10</v>
+        <v>3c</v>
       </c>
       <c r="C10">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D10">
         <f t="shared" ref="D10:K10" si="24">MOD(C10,D$2)</f>
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="E10">
         <f t="shared" si="24"/>
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="F10">
         <f t="shared" si="24"/>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H10">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I10">
         <f t="shared" si="24"/>
@@ -3120,7 +3120,7 @@
       </c>
       <c r="E15" s="2">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="35"/>
@@ -3221,11 +3221,11 @@
       </c>
       <c r="F16" s="2">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="37"/>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="39"/>
@@ -3322,7 +3322,7 @@
       </c>
       <c r="G17" s="2">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="39"/>
@@ -3334,7 +3334,7 @@
       </c>
       <c r="J17" s="2">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" si="39"/>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="E18" s="2">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="41"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="J18" s="2">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="2">
         <f t="shared" si="41"/>
@@ -3512,7 +3512,7 @@
       </c>
       <c r="F19" s="2">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="43"/>
@@ -3520,11 +3520,11 @@
       </c>
       <c r="H19" s="2">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="43"/>
@@ -29717,7 +29717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V256"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A139" workbookViewId="0">
       <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>

</xml_diff>